<commit_message>
renamed attributes for better clarification
</commit_message>
<xml_diff>
--- a/lab1/schema/data_dictionary.xlsx
+++ b/lab1/schema/data_dictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliannecrea/Desktop/jcrew/lab1/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JCHAO/Documents/UT/YEAR6/elem_data_jcrew/lab1/schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26620" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23160" windowHeight="20100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Country</t>
   </si>
@@ -95,15 +95,6 @@
     <t>acronym</t>
   </si>
   <si>
-    <t>ecf_code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>Ebola Treatment Centers or Units (ETCs or ETUs)</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t>Type: UN Agency, International NGO, Red Cross Movement, Government, Donors, Laboratory, International Organization, Private, National NGO, Other</t>
   </si>
   <si>
-    <t>Ebola Care Facility's identification code</t>
-  </si>
-  <si>
     <t>Respondent's identification code</t>
   </si>
   <si>
@@ -209,7 +197,16 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Q</t>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>org_name</t>
+  </si>
+  <si>
+    <t>org_type</t>
+  </si>
+  <si>
+    <t>Ebola Treatment Center / Ebola Care Facility's identification code</t>
   </si>
 </sst>
 </file>
@@ -587,7 +584,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,16 +596,16 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -624,7 +621,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -633,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -653,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -676,10 +673,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -699,10 +696,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -735,7 +732,7 @@
     </row>
     <row r="7" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>5</v>
@@ -744,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -764,10 +761,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -787,10 +784,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -810,10 +807,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -833,10 +830,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -856,10 +853,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -879,10 +876,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -897,17 +894,15 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -927,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -963,7 +958,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>14</v>
@@ -972,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -992,10 +987,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1015,10 +1010,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1038,10 +1033,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1061,10 +1056,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1084,10 +1079,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1107,10 +1102,10 @@
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1143,7 +1138,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>20</v>
@@ -1152,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -1172,10 +1167,10 @@
         <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -1192,13 +1187,13 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1215,13 +1210,13 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1238,13 +1233,13 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="11" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1261,13 +1256,13 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>

</xml_diff>

<commit_message>
updated data dictionary with new variable names from schemas
</commit_message>
<xml_diff>
--- a/lab1/schema/data_dictionary.xlsx
+++ b/lab1/schema/data_dictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JCHAO/Documents/UT/YEAR6/elem_data_jcrew/lab1/schema/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliannecrea/Desktop/jcrew/lab1/schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23160" windowHeight="20100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14520" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Country</t>
   </si>
@@ -50,12 +50,6 @@
     <t>etc_code</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>partner</t>
-  </si>
-  <si>
     <t>etc_name</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>acronym</t>
-  </si>
-  <si>
     <t>Ebola Treatment Centers or Units (ETCs or ETUs)</t>
   </si>
   <si>
@@ -207,6 +198,21 @@
   </si>
   <si>
     <t>Ebola Treatment Center / Ebola Care Facility's identification code</t>
+  </si>
+  <si>
+    <t>Country's name</t>
+  </si>
+  <si>
+    <t>partner_org</t>
+  </si>
+  <si>
+    <t>beds_open</t>
+  </si>
+  <si>
+    <t>Number of beds open</t>
+  </si>
+  <si>
+    <t>org_acronym</t>
   </si>
 </sst>
 </file>
@@ -581,31 +587,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -621,7 +627,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -630,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -645,15 +651,17 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -668,15 +676,17 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -691,15 +701,17 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -714,10 +726,18 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -730,41 +750,35 @@
       <c r="N6" s="8"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -779,15 +793,17 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -802,15 +818,17 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B10" s="11" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -825,15 +843,17 @@
       <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B11" s="11" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -848,15 +868,17 @@
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B12" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -871,15 +893,17 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B13" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -894,15 +918,17 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -917,15 +943,17 @@
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B15" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -940,10 +968,18 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -957,63 +993,59 @@
       <c r="O16" s="6"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1028,15 +1060,17 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B20" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1051,15 +1085,17 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B21" s="10" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1074,15 +1110,17 @@
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B22" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1097,15 +1135,17 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B23" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1120,10 +1160,18 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -1137,63 +1185,59 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1210,13 +1254,13 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1233,13 +1277,13 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1256,13 +1300,13 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -1277,21 +1321,67 @@
       <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated all data sets to have same attribute names as schemas, changed male/female to M/F, etc.
</commit_message>
<xml_diff>
--- a/lab1/schema/data_dictionary.xlsx
+++ b/lab1/schema/data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14520" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="10820" yWindow="460" windowWidth="14520" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>Country</t>
   </si>
@@ -197,9 +197,6 @@
     <t>org_type</t>
   </si>
   <si>
-    <t>Ebola Treatment Center / Ebola Care Facility's identification code</t>
-  </si>
-  <si>
     <t>Country's name</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>org_acronym</t>
+  </si>
+  <si>
+    <t>Ebola Care Facility's identification code</t>
   </si>
 </sst>
 </file>
@@ -589,15 +589,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -736,7 +734,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -847,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>23</v>
@@ -997,13 +995,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1252,9 +1250,11 @@
       <c r="O27" s="6"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B28" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>23</v>
@@ -1275,7 +1275,9 @@
       <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B29" s="11" t="s">
         <v>53</v>
       </c>
@@ -1298,7 +1300,9 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B30" s="11" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1310,7 @@
         <v>23</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -1321,7 +1325,9 @@
       <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B31" s="11" t="s">
         <v>54</v>
       </c>
@@ -1344,7 +1350,9 @@
       <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B32" s="11" t="s">
         <v>55</v>
       </c>

</xml_diff>